<commit_message>
add comment and change name
</commit_message>
<xml_diff>
--- a/TestData/LoginExcel.xlsx
+++ b/TestData/LoginExcel.xlsx
@@ -30,7 +30,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Krish</t>
+    <t>Muthu</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>